<commit_message>
All the statistics in the study
</commit_message>
<xml_diff>
--- a/Data_Statistics.xlsx
+++ b/Data_Statistics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\1 Drought in Korea\4 Figures\Fig. SEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65D64DB-8DAB-4F81-BBFF-C26F82C2E62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B38CED-667D-45A5-9C65-F1A60564246A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="note" sheetId="3" r:id="rId1"/>
@@ -289,14 +289,6 @@
   </si>
   <si>
     <t>Irrigated agriculture water use efficiency (DPRK)</t>
-  </si>
-  <si>
-    <t>Land area equipped for irrigation
-(DPRK)</t>
-  </si>
-  <si>
-    <t>Land area equipped for irrigation
-(ROK)</t>
   </si>
   <si>
     <t>Total dam capacity
@@ -692,6 +684,14 @@
       </rPr>
       <t>GWh</t>
     </r>
+  </si>
+  <si>
+    <t>Cropland equipped for irrigation
+(DPRK)</t>
+  </si>
+  <si>
+    <t>Cropland equipped for irrigation
+(ROK)</t>
   </si>
 </sst>
 </file>
@@ -1462,22 +1462,22 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -10864,7 +10864,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AK1" sqref="AK1"/>
+      <selection pane="topRight" activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -10929,267 +10929,267 @@
         <v>70</v>
       </c>
       <c r="F1" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="H1" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="I1" s="24" t="s">
         <v>74</v>
-      </c>
-      <c r="H1" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="I1" s="24" t="s">
-        <v>76</v>
       </c>
       <c r="J1" s="24" t="s">
         <v>72</v>
       </c>
       <c r="K1" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="L1" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="M1" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="N1" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="O1" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="M1" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="N1" s="24" t="s">
+      <c r="P1" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="O1" s="24" t="s">
+      <c r="Q1" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="P1" s="24" t="s">
+      <c r="R1" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="S1" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="Q1" s="24" t="s">
+      <c r="T1" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="U1" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="R1" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="S1" s="24" t="s">
+      <c r="V1" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="T1" s="24" t="s">
+      <c r="W1" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="X1" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y1" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="U1" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="V1" s="24" t="s">
+      <c r="Z1" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="AA1" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="AB1" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="W1" s="24" t="s">
+      <c r="AC1" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="X1" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y1" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="Z1" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="AA1" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="AB1" s="24" t="s">
+      <c r="AD1" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="AC1" s="25" t="s">
+      <c r="AE1" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="AD1" s="24" t="s">
+      <c r="AF1" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="AG1" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="AH1" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI1" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="AJ1" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK1" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="AL1" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="AE1" s="24" t="s">
+      <c r="AM1" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="AF1" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="AG1" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="AH1" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="AI1" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="AJ1" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="AK1" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="AL1" s="24" t="s">
+      <c r="AN1" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="AM1" s="24" t="s">
+      <c r="AO1" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="AN1" s="24" t="s">
+      <c r="AP1" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="AO1" s="24" t="s">
+      <c r="AQ1" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="AP1" s="24" t="s">
+      <c r="AR1" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="AQ1" s="24" t="s">
+      <c r="AS1" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="AR1" s="24" t="s">
+      <c r="AT1" s="24" t="s">
         <v>98</v>
-      </c>
-      <c r="AS1" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="AT1" s="24" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:46" s="26" customFormat="1" ht="18">
       <c r="A2" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="E2" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="G2" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="H2" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="J2" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="K2" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="L2" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="M2" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="N2" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="O2" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="P2" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q2" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="R2" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="S2" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="T2" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="U2" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="V2" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="W2" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="X2" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="Y2" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z2" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="AA2" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB2" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="AC2" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="AD2" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="AE2" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="AF2" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="AG2" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="H2" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="I2" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="J2" s="28" t="s">
-        <v>121</v>
-      </c>
-      <c r="K2" s="28" t="s">
-        <v>121</v>
-      </c>
-      <c r="L2" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="M2" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="N2" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O2" s="28" t="s">
-        <v>124</v>
-      </c>
-      <c r="P2" s="28" t="s">
+      <c r="AH2" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="AI2" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="Q2" s="28" t="s">
+      <c r="AJ2" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="AK2" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="AL2" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="R2" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="S2" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="T2" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="U2" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="V2" s="28" t="s">
-        <v>124</v>
-      </c>
-      <c r="W2" s="28" t="s">
+      <c r="AM2" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="X2" s="28" t="s">
+      <c r="AN2" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="AO2" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="AP2" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="AQ2" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="Y2" s="28" t="s">
+      <c r="AR2" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="Z2" s="28" t="s">
+      <c r="AS2" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="AA2" s="28" t="s">
+      <c r="AT2" s="28" t="s">
         <v>127</v>
-      </c>
-      <c r="AB2" s="28" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC2" s="28" t="s">
-        <v>127</v>
-      </c>
-      <c r="AD2" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="AE2" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="AF2" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="AG2" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH2" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="AI2" s="28" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ2" s="28" t="s">
-        <v>127</v>
-      </c>
-      <c r="AK2" s="28" t="s">
-        <v>127</v>
-      </c>
-      <c r="AL2" s="28" t="s">
-        <v>128</v>
-      </c>
-      <c r="AM2" s="28" t="s">
-        <v>128</v>
-      </c>
-      <c r="AN2" s="28" t="s">
-        <v>128</v>
-      </c>
-      <c r="AO2" s="28" t="s">
-        <v>128</v>
-      </c>
-      <c r="AP2" s="28" t="s">
-        <v>128</v>
-      </c>
-      <c r="AQ2" s="28" t="s">
-        <v>129</v>
-      </c>
-      <c r="AR2" s="28" t="s">
-        <v>129</v>
-      </c>
-      <c r="AS2" s="28" t="s">
-        <v>129</v>
-      </c>
-      <c r="AT2" s="28" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:46">

</xml_diff>